<commit_message>
changes to result and search
</commit_message>
<xml_diff>
--- a/db_excel.xlsx
+++ b/db_excel.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Documentos\Proyectos\manga-peru\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Documents\GitHub\tiendas_manga_peru\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4E1754-79A0-4331-9452-9221F212D8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tiendas" sheetId="1" r:id="rId1"/>
+    <sheet name="provincia" sheetId="2" r:id="rId1"/>
+    <sheet name="distrito" sheetId="3" r:id="rId2"/>
+    <sheet name="tiendas" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>id_store</t>
   </si>
@@ -54,16 +57,105 @@
   </si>
   <si>
     <t>urlWeb</t>
+  </si>
+  <si>
+    <t>id_ref</t>
+  </si>
+  <si>
+    <t>id_dist</t>
+  </si>
+  <si>
+    <t>LIMA</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>https://lustyweaboo.tiendada.com/</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>lusty.weaboo@gmail.com</t>
+  </si>
+  <si>
+    <t>Somos una tienda digital importadora de Hentai y Doujinshis de Japón a Perú, también podemos realizar pedidos de distintas paginas de Japón y subastas de yahoo auctions</t>
+  </si>
+  <si>
+    <t>Lusty Weaboo</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/lusty.weaboo</t>
+  </si>
+  <si>
+    <t>lustyweaboo.png</t>
+  </si>
+  <si>
+    <t>Lin's Store</t>
+  </si>
+  <si>
+    <t>Figuras, libros, discos y goods originales (Japón, Corea del Sur, Taiwán, USA y China) en pre orden, stock o a pedido.</t>
+  </si>
+  <si>
+    <t>linstore.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Linstorex3</t>
+  </si>
+  <si>
+    <t>Skips Store</t>
+  </si>
+  <si>
+    <t>Mangabo Perú</t>
+  </si>
+  <si>
+    <t>mangaboperu.jpg</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/MangaboPeru</t>
+  </si>
+  <si>
+    <t>mangaboperu@gmail.com</t>
+  </si>
+  <si>
+    <t>Mangas en stock y a pedido</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d15607.644325114652!2d-77.0391241792354!3d-12.049638778429935!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x9105c8b7076ce525%3A0xe68c998a917d5075!2sCercado%20de%20Lima%2015001!5e0!3m2!1ses-419!2spe!4v1660233071476!5m2!1ses-419!2spe</t>
+  </si>
+  <si>
+    <t>skipsstore@hotmail.com</t>
+  </si>
+  <si>
+    <t>skipsstoreperu.com</t>
+  </si>
+  <si>
+    <t>skipsstore.png</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/profile.php?id=100065507559327</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,13 +178,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,52 +468,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B38716B7-EFE6-43D4-B349-6BFBA2B8D61A}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9077BF3-BB94-4D24-83E1-9B47E35651B1}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>934902565</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>987654321</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>943811106</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>973379797</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{9FCFBD49-F073-4056-B4B6-8A1E843DDE01}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{69C1B81F-C2CE-442F-8DA6-E4D92BE4CE30}"/>
+    <hyperlink ref="I2" r:id="rId3" xr:uid="{F839F2D8-CCC1-4910-A7E7-83BB846D3881}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{E36496F6-5CC0-41E4-9D29-6C5F3E7FB1AB}"/>
+    <hyperlink ref="I4" r:id="rId5" xr:uid="{7579626A-76BD-4B46-896C-F6AF5B57F03B}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{3EDAD2D0-6466-49D3-9279-CA7DE0874ADB}"/>
+    <hyperlink ref="K4" r:id="rId7" display="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d15607.644325114652!2d-77.0391241792354!3d-12.049638778429935!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x9105c8b7076ce525%3A0xe68c998a917d5075!2sCercado%20de%20Lima%2015001!5e0!3m2!1ses-419!2spe!4v1660233071476!5m2!1ses-419!2spe" xr:uid="{DC349C50-6FAF-4606-BE07-F82A552F188D}"/>
+    <hyperlink ref="H5" r:id="rId8" xr:uid="{36FA8E14-427F-47AC-8C70-1E55311B0530}"/>
+    <hyperlink ref="I5" r:id="rId9" xr:uid="{B8536CFA-5C7B-4939-9ECC-60EFB414EC8C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Search added and dropdowns logic changed
</commit_message>
<xml_diff>
--- a/db_excel.xlsx
+++ b/db_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Documents\GitHub\tiendas_manga_peru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4E1754-79A0-4331-9452-9221F212D8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4437941-9C5D-4AA1-9771-11C5BD800DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>id_store</t>
   </si>
@@ -138,6 +138,34 @@
   </si>
   <si>
     <t>https://www.facebook.com/profile.php?id=100065507559327</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/Dragonay</t>
+  </si>
+  <si>
+    <t>Colecciones Dragonay</t>
+  </si>
+  <si>
+    <t>Somos Distribuidores de 2 marcas reconocidas Panini Perú y DKV
+vendemos Mangas de tus animes</t>
+  </si>
+  <si>
+    <t>arenales.dragonay@gmail.com</t>
+  </si>
+  <si>
+    <t>tiktok.com/@colecciones_dragonay</t>
+  </si>
+  <si>
+    <t>dragonay.jpg</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Av Arenales 1737, tienda 1-11 (sotano), Lince- Lima, Lince, Peru, 15073</t>
+  </si>
+  <si>
+    <t>id_provi</t>
   </si>
 </sst>
 </file>
@@ -549,25 +577,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,184 +603,243 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>101</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
         <v>934902565</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>101</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
         <v>987654321</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="1"/>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>101</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
         <v>943811106</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>101</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
         <v>973379797</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>35</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>34</v>
       </c>
-      <c r="M5" t="s">
-        <v>13</v>
+      <c r="N5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>116</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>928763812</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{9FCFBD49-F073-4056-B4B6-8A1E843DDE01}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{69C1B81F-C2CE-442F-8DA6-E4D92BE4CE30}"/>
-    <hyperlink ref="I2" r:id="rId3" xr:uid="{F839F2D8-CCC1-4910-A7E7-83BB846D3881}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{E36496F6-5CC0-41E4-9D29-6C5F3E7FB1AB}"/>
-    <hyperlink ref="I4" r:id="rId5" xr:uid="{7579626A-76BD-4B46-896C-F6AF5B57F03B}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{3EDAD2D0-6466-49D3-9279-CA7DE0874ADB}"/>
-    <hyperlink ref="K4" r:id="rId7" display="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d15607.644325114652!2d-77.0391241792354!3d-12.049638778429935!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x9105c8b7076ce525%3A0xe68c998a917d5075!2sCercado%20de%20Lima%2015001!5e0!3m2!1ses-419!2spe!4v1660233071476!5m2!1ses-419!2spe" xr:uid="{DC349C50-6FAF-4606-BE07-F82A552F188D}"/>
-    <hyperlink ref="H5" r:id="rId8" xr:uid="{36FA8E14-427F-47AC-8C70-1E55311B0530}"/>
-    <hyperlink ref="I5" r:id="rId9" xr:uid="{B8536CFA-5C7B-4939-9ECC-60EFB414EC8C}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{9FCFBD49-F073-4056-B4B6-8A1E843DDE01}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{69C1B81F-C2CE-442F-8DA6-E4D92BE4CE30}"/>
+    <hyperlink ref="J2" r:id="rId3" xr:uid="{F839F2D8-CCC1-4910-A7E7-83BB846D3881}"/>
+    <hyperlink ref="J3" r:id="rId4" xr:uid="{E36496F6-5CC0-41E4-9D29-6C5F3E7FB1AB}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{7579626A-76BD-4B46-896C-F6AF5B57F03B}"/>
+    <hyperlink ref="I4" r:id="rId6" xr:uid="{3EDAD2D0-6466-49D3-9279-CA7DE0874ADB}"/>
+    <hyperlink ref="L4" r:id="rId7" display="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d15607.644325114652!2d-77.0391241792354!3d-12.049638778429935!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x9105c8b7076ce525%3A0xe68c998a917d5075!2sCercado%20de%20Lima%2015001!5e0!3m2!1ses-419!2spe!4v1660233071476!5m2!1ses-419!2spe" xr:uid="{DC349C50-6FAF-4606-BE07-F82A552F188D}"/>
+    <hyperlink ref="I5" r:id="rId8" xr:uid="{36FA8E14-427F-47AC-8C70-1E55311B0530}"/>
+    <hyperlink ref="J5" r:id="rId9" xr:uid="{B8536CFA-5C7B-4939-9ECC-60EFB414EC8C}"/>
+    <hyperlink ref="J6" r:id="rId10" xr:uid="{54C65139-D463-4D9B-A206-A273AF8CB2B1}"/>
+    <hyperlink ref="I6" r:id="rId11" xr:uid="{B3A7B542-976B-497F-899B-62AB77B8AE8F}"/>
+    <hyperlink ref="M6" r:id="rId12" xr:uid="{1B2F4BF0-C697-4782-B170-A83CCCF418DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>